<commit_message>
fix: Database 컬럼 수정
</commit_message>
<xml_diff>
--- a/documents/note-테이블명세(2022-12-25).xlsx
+++ b/documents/note-테이블명세(2022-12-25).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Project\Project_Note\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40E360E-0EF5-48A5-A5F7-0D800D94C33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7731BD13-C878-4A4B-90C4-CDE709C09389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="2205" windowWidth="27855" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="사용자정보" sheetId="11" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="194">
   <si>
     <t>열 이름</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -407,20 +407,12 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>배경음악</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>fk_subkey</t>
   </si>
   <si>
     <t>fk_catsub</t>
   </si>
   <si>
-    <t>DEFAULT 1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>다크모드</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -466,10 +458,6 @@
   </si>
   <si>
     <t>tbl_score</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>u_bgm</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -823,6 +811,22 @@
   </si>
   <si>
     <t>u_darkmode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>키워드 수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_keycount</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제 수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>c_subcount</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1442,7 +1446,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1578,33 +1582,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1673,6 +1650,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2019,7 +2002,7 @@
   <dimension ref="B1:L35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2675,22 +2658,22 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="59" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60">
+      <c r="I2" s="50"/>
+      <c r="J2" s="51">
         <v>44575</v>
       </c>
-      <c r="K2" s="61"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="28" t="s">
         <v>11</v>
       </c>
@@ -2700,38 +2683,38 @@
         <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="62" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63" t="s">
+      <c r="I3" s="53"/>
+      <c r="J3" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="64"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="16"/>
     </row>
     <row r="4" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="56"/>
+      <c r="C4" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
@@ -2773,13 +2756,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>38</v>
@@ -2794,7 +2777,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="30"/>
       <c r="L6" s="31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -2802,13 +2785,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>103</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>38</v>
@@ -2827,13 +2810,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>106</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>38</v>
@@ -2842,7 +2825,7 @@
         <v>31</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -2854,13 +2837,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>38</v>
@@ -2877,13 +2860,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>38</v>
@@ -2900,16 +2883,16 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>31</v>
@@ -2926,14 +2909,14 @@
       <c r="B12" s="8">
         <v>7</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>93</v>
+      <c r="C12" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>109</v>
+        <v>189</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>82</v>
@@ -2942,7 +2925,7 @@
         <v>31</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -2955,30 +2938,18 @@
       <c r="B13" s="8">
         <v>8</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>81</v>
-      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="44"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="31" t="s">
-        <v>87</v>
-      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="14"/>
     </row>
     <row r="14" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="8">
@@ -2986,12 +2957,10 @@
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
@@ -3922,22 +3891,22 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="59" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60">
+      <c r="I2" s="50"/>
+      <c r="J2" s="51">
         <v>44575</v>
       </c>
-      <c r="K2" s="61"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="28" t="s">
         <v>11</v>
       </c>
@@ -3947,38 +3916,38 @@
         <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63" t="s">
+      <c r="I3" s="53"/>
+      <c r="J3" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="64"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="16"/>
     </row>
     <row r="4" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="56"/>
+      <c r="C4" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
@@ -4020,13 +3989,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>38</v>
@@ -4049,13 +4018,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>38</v>
@@ -4065,16 +4034,16 @@
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="L7" s="31" t="s">
         <v>116</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="L7" s="31" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="24" x14ac:dyDescent="0.15">
@@ -4082,13 +4051,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="27" t="s">
         <v>112</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>115</v>
       </c>
       <c r="F8" s="27" t="s">
         <v>29</v>
@@ -4112,10 +4081,10 @@
         <v>60</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>29</v>
@@ -4125,7 +4094,7 @@
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>65</v>
@@ -4148,7 +4117,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>29</v>
@@ -4167,16 +4136,16 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>78</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>31</v>
@@ -4193,14 +4162,14 @@
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="65" t="s">
-        <v>190</v>
-      </c>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="67"/>
+      <c r="E12" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="58"/>
       <c r="I12" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -4212,10 +4181,10 @@
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="70"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="61"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -4227,13 +4196,13 @@
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="70"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="14"/>
@@ -4244,10 +4213,10 @@
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="70"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="61"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -4259,10 +4228,10 @@
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="73"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="64"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
@@ -4291,7 +4260,7 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -4510,7 +4479,7 @@
   <dimension ref="B1:L35"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E9" sqref="E9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5168,20 +5137,20 @@
       <c r="C2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="59" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60">
+      <c r="I2" s="50"/>
+      <c r="J2" s="51">
         <v>44918</v>
       </c>
-      <c r="K2" s="61"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="28" t="s">
         <v>11</v>
       </c>
@@ -5193,36 +5162,36 @@
       <c r="C3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="62" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63" t="s">
+      <c r="I3" s="53"/>
+      <c r="J3" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="64"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="16"/>
     </row>
     <row r="4" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="56"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
@@ -5267,7 +5236,7 @@
         <v>60</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>63</v>
@@ -5293,13 +5262,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>38</v>
@@ -5311,16 +5280,16 @@
         <v>47</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K7" s="30" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -5343,7 +5312,7 @@
         <v>31</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="30"/>
@@ -5354,17 +5323,17 @@
       <c r="B9" s="8">
         <v>4</v>
       </c>
-      <c r="C9" s="30" t="s">
-        <v>84</v>
+      <c r="C9" s="9" t="s">
+        <v>192</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>86</v>
+        <v>193</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>31</v>
@@ -5375,26 +5344,36 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="30"/>
-      <c r="L9" s="31" t="s">
-        <v>87</v>
-      </c>
+      <c r="L9" s="31"/>
     </row>
     <row r="10" spans="2:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="8">
         <v>5</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="65" t="s">
-        <v>189</v>
-      </c>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="67"/>
+      <c r="C10" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="29"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="31" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="11" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="8">
@@ -5402,25 +5381,27 @@
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="70"/>
+      <c r="E11" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="58"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
-      <c r="L11" s="14"/>
+      <c r="L11" s="29"/>
     </row>
     <row r="12" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="8">
         <v>7</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="73"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="61"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -5431,11 +5412,11 @@
         <v>8</v>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="64"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -5619,7 +5600,7 @@
         <v>39</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
@@ -5640,7 +5621,7 @@
         <v>39</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -5730,13 +5711,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="E10:H12"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="E11:H13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5750,7 +5731,7 @@
   <dimension ref="B1:L35"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E12" sqref="E12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6408,20 +6389,20 @@
       <c r="C2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="59" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60">
+      <c r="I2" s="50"/>
+      <c r="J2" s="51">
         <v>44918</v>
       </c>
-      <c r="K2" s="61"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="28" t="s">
         <v>11</v>
       </c>
@@ -6433,36 +6414,36 @@
       <c r="C3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="62" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63" t="s">
+      <c r="I3" s="53"/>
+      <c r="J3" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="64"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="16"/>
     </row>
     <row r="4" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="56"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
@@ -6507,7 +6488,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>61</v>
@@ -6561,7 +6542,7 @@
         <v>60</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>62</v>
@@ -6576,7 +6557,7 @@
         <v>47</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>65</v>
@@ -6668,16 +6649,16 @@
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>77</v>
+        <v>190</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>78</v>
+        <v>154</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>79</v>
+        <v>191</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>31</v>
@@ -6688,53 +6669,59 @@
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
-      <c r="L12" s="14" t="s">
-        <v>80</v>
-      </c>
+      <c r="L12" s="14"/>
     </row>
     <row r="13" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="8">
         <v>8</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>178</v>
+        <v>77</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>157</v>
+        <v>78</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>179</v>
+        <v>79</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="G13" s="9"/>
+        <v>82</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="H13" s="9" t="s">
         <v>81</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
-      <c r="L13" s="14"/>
+      <c r="L13" s="14" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="8">
         <v>9</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>26</v>
+        <v>154</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+        <v>155</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
@@ -6744,14 +6731,20 @@
       <c r="B15" s="8">
         <v>10</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="47"/>
+      <c r="C15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -6763,10 +6756,12 @@
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="49"/>
+      <c r="E16" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="58"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
@@ -6778,10 +6773,10 @@
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="52"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="61"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
@@ -6793,10 +6788,10 @@
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="64"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
@@ -6884,7 +6879,7 @@
         <v>39</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -6999,7 +6994,8 @@
       <c r="L35" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="E16:H18"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:I2"/>
@@ -7677,20 +7673,20 @@
       <c r="C2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="59" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60">
+      <c r="I2" s="50"/>
+      <c r="J2" s="51">
         <v>44918</v>
       </c>
-      <c r="K2" s="61"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="28" t="s">
         <v>11</v>
       </c>
@@ -7702,36 +7698,36 @@
       <c r="C3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="62" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63" t="s">
+      <c r="I3" s="53"/>
+      <c r="J3" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="64"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="16"/>
     </row>
     <row r="4" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="56"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
@@ -7776,7 +7772,7 @@
         <v>69</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>70</v>
@@ -7805,7 +7801,7 @@
         <v>59</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>66</v>
@@ -7820,7 +7816,7 @@
         <v>47</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>64</v>
@@ -7837,16 +7833,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>78</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>31</v>
@@ -7911,12 +7907,12 @@
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="65" t="s">
-        <v>145</v>
-      </c>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="67"/>
+      <c r="E11" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="58"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -7928,10 +7924,10 @@
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="70"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -7943,10 +7939,10 @@
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="73"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="64"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -8130,7 +8126,7 @@
         <v>39</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
@@ -8911,20 +8907,20 @@
       <c r="C2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="59" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60">
+      <c r="I2" s="50"/>
+      <c r="J2" s="51">
         <v>44918</v>
       </c>
-      <c r="K2" s="61"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="28" t="s">
         <v>11</v>
       </c>
@@ -8936,36 +8932,36 @@
       <c r="C3" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="62" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63" t="s">
+      <c r="I3" s="53"/>
+      <c r="J3" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="64"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="16"/>
     </row>
     <row r="4" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="56"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
@@ -9010,7 +9006,7 @@
         <v>71</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>72</v>
@@ -9039,10 +9035,10 @@
         <v>59</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>38</v>
@@ -9054,7 +9050,7 @@
         <v>47</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>64</v>
@@ -9131,7 +9127,7 @@
         <v>37</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>38</v>
@@ -9156,7 +9152,7 @@
         <v>37</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>38</v>
@@ -9201,12 +9197,12 @@
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="65" t="s">
-        <v>153</v>
-      </c>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="67"/>
+      <c r="E13" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="58"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -9218,10 +9214,10 @@
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="70"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
@@ -9233,10 +9229,10 @@
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="70"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="61"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -9496,7 +9492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABF5D82-5A29-40C3-8037-DD259C776DB2}">
   <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -10153,22 +10149,22 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D2" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="59" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60">
+      <c r="I2" s="50"/>
+      <c r="J2" s="51">
         <v>44986</v>
       </c>
-      <c r="K2" s="61"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="28" t="s">
         <v>11</v>
       </c>
@@ -10178,38 +10174,38 @@
         <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="62" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63" t="s">
+      <c r="I3" s="53"/>
+      <c r="J3" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="64"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="16"/>
     </row>
     <row r="4" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="55" t="s">
-        <v>164</v>
-      </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="56"/>
+      <c r="C4" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
@@ -10251,21 +10247,21 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="45" t="s">
         <v>47</v>
       </c>
       <c r="I6" s="3"/>
@@ -10278,13 +10274,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>38</v>
@@ -10296,16 +10292,16 @@
         <v>47</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K7" s="30" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -10319,7 +10315,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>28</v>
@@ -10346,7 +10342,7 @@
         <v>24</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>28</v>
@@ -10373,7 +10369,7 @@
         <v>37</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>38</v>
@@ -10392,13 +10388,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>28</v>
@@ -10417,26 +10413,26 @@
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>78</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>28</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="29" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -10444,13 +10440,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>28</v>
@@ -10469,13 +10465,13 @@
         <v>9</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>28</v>
@@ -10495,11 +10491,11 @@
       </c>
       <c r="C15" s="32"/>
       <c r="D15" s="32"/>
-      <c r="E15" s="65" t="s">
-        <v>191</v>
-      </c>
-      <c r="F15" s="66"/>
-      <c r="G15" s="67"/>
+      <c r="E15" s="56" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" s="57"/>
+      <c r="G15" s="58"/>
       <c r="H15" s="32"/>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -10512,9 +10508,9 @@
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="32"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="73"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="64"/>
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -10741,13 +10737,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="E15:G16"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="E15:G16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11417,22 +11413,22 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D2" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="59" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60">
+      <c r="I2" s="50"/>
+      <c r="J2" s="51">
         <v>44575</v>
       </c>
-      <c r="K2" s="61"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="28" t="s">
         <v>11</v>
       </c>
@@ -11442,38 +11438,38 @@
         <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="62" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63" t="s">
+      <c r="I3" s="53"/>
+      <c r="J3" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="64"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="16"/>
     </row>
     <row r="4" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="55" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="56"/>
+      <c r="C4" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
@@ -11515,19 +11511,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>131</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -11540,26 +11536,26 @@
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="30"/>
       <c r="L7" s="31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -11567,19 +11563,19 @@
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>78</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H8" s="37" t="s">
         <v>47</v>
@@ -11588,7 +11584,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="30"/>
       <c r="L8" s="31" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -11597,12 +11593,12 @@
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="74" t="s">
-        <v>138</v>
-      </c>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="76"/>
+      <c r="E9" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="67"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>

</xml_diff>

<commit_message>
fix: Chart 데이터 수정
</commit_message>
<xml_diff>
--- a/documents/note-테이블명세(2022-12-25).xlsx
+++ b/documents/note-테이블명세(2022-12-25).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Project\Project_Note\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMS50520\Documents\workspace\Project\NoteIT\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCBDD63-4C66-400A-83A4-63F50AA03D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E358F49-9710-447B-AA91-2FA54E83D6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2835" windowWidth="27855" windowHeight="13200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1680" windowWidth="27690" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="사용자정보" sheetId="11" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="202">
   <si>
     <t>열 이름</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -446,10 +446,6 @@
   </si>
   <si>
     <t>날짜</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>점수</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -611,13 +607,6 @@
   </si>
   <si>
     <t>a_subid</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRIMARY KEY(a_attid, a_subid),
-CONSTRAINT fk_subatt
-FOREIGN KEY(a_subid) REFERENCES tbl_subjects(s_subid)
-ON DELETE CASCADE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -815,10 +804,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>u_totalscore</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>퀴즈일자</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -848,6 +833,29 @@
   </si>
   <si>
     <t>tbl_scores</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 득점</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 총점</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sc_totalscore</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRIMARY KEY(a_attid),
+CONSTRAINT fk_subatt
+FOREIGN KEY(a_subid) REFERENCES tbl_subjects(s_subid)
+ON DELETE CASCADE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>u_score</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1456,7 +1464,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1657,6 +1665,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2002,8 +2013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B2AE80-C225-4A09-A24A-B47819C21C0A}">
   <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2684,7 +2695,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D3" s="48"/>
       <c r="E3" s="48"/>
@@ -2757,13 +2768,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>38</v>
@@ -2778,7 +2789,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="30"/>
       <c r="L6" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -2826,7 +2837,7 @@
         <v>31</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -2838,13 +2849,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>38</v>
@@ -2861,13 +2872,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>38</v>
@@ -2887,13 +2898,13 @@
         <v>95</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>31</v>
@@ -2913,7 +2924,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -3222,7 +3233,7 @@
   <dimension ref="B1:L35"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3903,7 +3914,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D3" s="48"/>
       <c r="E3" s="48"/>
@@ -3924,7 +3935,7 @@
         <v>43</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" s="45"/>
       <c r="E4" s="45"/>
@@ -3976,13 +3987,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>38</v>
@@ -4005,13 +4016,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>38</v>
@@ -4021,16 +4032,16 @@
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="24" x14ac:dyDescent="0.15">
@@ -4044,7 +4055,7 @@
         <v>102</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" s="27" t="s">
         <v>29</v>
@@ -4065,13 +4076,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>102</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F9" s="27" t="s">
         <v>29</v>
@@ -4092,13 +4103,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>102</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>29</v>
@@ -4125,7 +4136,7 @@
         <v>98</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>29</v>
@@ -4135,7 +4146,7 @@
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>64</v>
@@ -4158,7 +4169,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>29</v>
@@ -4177,13 +4188,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>104</v>
+        <v>197</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>77</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>94</v>
@@ -4201,17 +4212,23 @@
       <c r="B14" s="8">
         <v>9</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="9" t="s">
-        <v>114</v>
-      </c>
+      <c r="C14" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="14"/>
@@ -4222,10 +4239,12 @@
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="60"/>
+      <c r="E15" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="57"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -4238,12 +4257,12 @@
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="58"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
       <c r="H16" s="60"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="14"/>
@@ -4254,10 +4273,10 @@
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="60"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="63"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
@@ -4269,7 +4288,7 @@
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E18" s="44"/>
       <c r="F18" s="44"/>
@@ -4470,13 +4489,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="E14:H17"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="E15:H17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5273,13 +5292,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>38</v>
@@ -5291,16 +5310,16 @@
         <v>47</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K7" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -5323,7 +5342,7 @@
         <v>31</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="30"/>
@@ -5335,16 +5354,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>31</v>
@@ -5368,7 +5387,7 @@
         <v>83</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>81</v>
@@ -5391,13 +5410,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>28</v>
@@ -5418,13 +5437,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>28</v>
@@ -5445,7 +5464,7 @@
       <c r="C13" s="9"/>
       <c r="D13" s="32"/>
       <c r="E13" s="58" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F13" s="59"/>
       <c r="G13" s="59"/>
@@ -5633,7 +5652,7 @@
         <v>39</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
@@ -5654,7 +5673,7 @@
         <v>39</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -5675,7 +5694,7 @@
         <v>39</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
@@ -5771,8 +5790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6640,7 +6659,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>24</v>
@@ -6667,16 +6686,16 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>31</v>
@@ -6748,7 +6767,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F14" s="56"/>
       <c r="G14" s="56"/>
@@ -7846,13 +7865,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>77</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>94</v>
@@ -7871,16 +7890,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>31</v>
@@ -7948,7 +7967,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F12" s="56"/>
       <c r="G12" s="56"/>
@@ -8145,13 +8164,13 @@
         <v>2</v>
       </c>
       <c r="C28" s="43" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D28" s="21" t="s">
         <v>39</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
@@ -8172,7 +8191,7 @@
         <v>39</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -8282,7 +8301,7 @@
   <dimension ref="B1:L35"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9071,7 +9090,7 @@
         <v>98</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>38</v>
@@ -9079,11 +9098,9 @@
       <c r="G7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="37" t="s">
-        <v>47</v>
-      </c>
+      <c r="H7" s="37"/>
       <c r="I7" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>63</v>
@@ -9160,7 +9177,7 @@
         <v>37</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>38</v>
@@ -9185,7 +9202,7 @@
         <v>37</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>38</v>
@@ -9231,7 +9248,7 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="55" t="s">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="F13" s="56"/>
       <c r="G13" s="56"/>
@@ -10182,7 +10199,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D2" s="47" t="s">
         <v>14</v>
@@ -10207,7 +10224,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D3" s="48"/>
       <c r="E3" s="48"/>
@@ -10228,7 +10245,7 @@
         <v>43</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" s="45"/>
       <c r="E4" s="45"/>
@@ -10280,19 +10297,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="H6" s="42" t="s">
         <v>47</v>
@@ -10307,13 +10324,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>38</v>
@@ -10325,16 +10342,16 @@
         <v>47</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K7" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -10348,7 +10365,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>28</v>
@@ -10375,7 +10392,7 @@
         <v>24</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>28</v>
@@ -10402,7 +10419,7 @@
         <v>37</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>38</v>
@@ -10421,13 +10438,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>28</v>
@@ -10446,26 +10463,26 @@
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>77</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>28</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -10473,13 +10490,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>28</v>
@@ -10498,13 +10515,13 @@
         <v>9</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>28</v>
@@ -10525,7 +10542,7 @@
       <c r="C15" s="32"/>
       <c r="D15" s="32"/>
       <c r="E15" s="55" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F15" s="56"/>
       <c r="G15" s="57"/>
@@ -11446,7 +11463,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" s="47" t="s">
         <v>14</v>
@@ -11471,7 +11488,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" s="48"/>
       <c r="E3" s="48"/>
@@ -11492,7 +11509,7 @@
         <v>43</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="45"/>
       <c r="E4" s="45"/>
@@ -11544,19 +11561,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -11569,26 +11586,26 @@
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="F7" s="27" t="s">
+      <c r="G7" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="30"/>
       <c r="L7" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -11602,13 +11619,13 @@
         <v>77</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>94</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H8" s="37" t="s">
         <v>47</v>
@@ -11617,7 +11634,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="30"/>
       <c r="L8" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -11627,7 +11644,7 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" s="65"/>
       <c r="G9" s="65"/>

</xml_diff>